<commit_message>
BOM updated to correct errors & changed starting hardware test
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bb7136279314008f/Uni_PC_backup/Y4S2/EE579/Assignment/EE579-Skittles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{5403E067-3A5D-4EEF-A823-00EBFBF2B18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70DDF23C-997F-4726-A061-1A1CC26998C2}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{5403E067-3A5D-4EEF-A823-00EBFBF2B18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F79301D4-3D17-4480-B6ED-16E42C302350}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1006,16 +1006,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1031,6 +1024,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -1038,9 +1038,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.000"/>
     </dxf>
@@ -1062,6 +1059,9 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1075,25 +1075,29 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F2573AAE-30E1-4A8B-A87C-53D85222EA60}" name="Table2" displayName="Table2" ref="B1:O56" totalsRowCount="1" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F2573AAE-30E1-4A8B-A87C-53D85222EA60}" name="Table2" displayName="Table2" ref="B1:O56" totalsRowCount="1" headerRowDxfId="7">
   <autoFilter ref="B1:O55" xr:uid="{F2573AAE-30E1-4A8B-A87C-53D85222EA60}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{D9D53CF3-8476-45FC-9926-772D8655B7FF}" name="Component ID" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{A24948CA-1610-48CB-B980-9AA81C1A233D}" name="Name"/>
     <tableColumn id="3" xr3:uid="{1580CE8E-C185-41E3-9040-FFDCE18C32D9}" name="Type"/>
-    <tableColumn id="4" xr3:uid="{740C0ED2-BD84-4B54-938C-65AC3CA420A1}" name="Quantity" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{740C0ED2-BD84-4B54-938C-65AC3CA420A1}" name="Quantity" dataDxfId="6" totalsRowDxfId="2"/>
     <tableColumn id="15" xr3:uid="{BFBD9B3A-2E94-4AEB-A8B3-D19C2DD2ABAA}" name="PCB Designator(s)"/>
     <tableColumn id="5" xr3:uid="{C2711204-1624-4B74-ADF6-5D5F69404247}" name="Package"/>
     <tableColumn id="6" xr3:uid="{B3B79F3A-5B27-46FF-8AB8-397028BF404B}" name="Manufacturer"/>
     <tableColumn id="7" xr3:uid="{F6E35C8E-126C-40DA-9391-0244AEEEF05F}" name="Manufacurer Part Number"/>
     <tableColumn id="11" xr3:uid="{F73DCBB8-C4CB-4DCC-ACDA-6D534FB6177E}" name="Distributer"/>
     <tableColumn id="12" xr3:uid="{5A30FE29-69B5-4505-B406-82F04F2FD311}" name="Distributer Stock Number"/>
-    <tableColumn id="9" xr3:uid="{9D4F6498-797D-4325-95B9-F51CC78E5A45}" name="Individual Cost (inc VAT) (£)" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{06C4749E-89A3-4023-9714-C0AB173CC833}" name="Total Cost (£)" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="2">
+    <tableColumn id="9" xr3:uid="{9D4F6498-797D-4325-95B9-F51CC78E5A45}" name="Individual Cost (inc VAT) (£)" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{06C4749E-89A3-4023-9714-C0AB173CC833}" name="Total Cost (£)" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="1">
       <calculatedColumnFormula>Table2[[#This Row],[Individual Cost (inc VAT) (£)]]*Table2[[#This Row],[Quantity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{08B5C1FA-5F70-407E-916F-794B7583F777}" name="Note" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{08B5C1FA-5F70-407E-916F-794B7583F777}" name="Note" dataDxfId="3" totalsRowDxfId="0"/>
     <tableColumn id="13" xr3:uid="{0D537E1A-943B-495D-8650-357F684B1418}" name="Link"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1365,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1379,7 @@
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -1389,51 +1393,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="13" t="s">
         <v>163</v>
       </c>
       <c r="B2" t="s">
@@ -1445,7 +1449,7 @@
       <c r="D2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
       <c r="F2" t="s">
@@ -1481,7 +1485,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="15"/>
       <c r="B3" t="s">
         <v>180</v>
       </c>
@@ -1491,7 +1495,7 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>1</v>
       </c>
       <c r="F3" t="s">
@@ -1525,7 +1529,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="15"/>
       <c r="B4" t="s">
         <v>181</v>
       </c>
@@ -1535,7 +1539,7 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>9</v>
       </c>
       <c r="F4" t="s">
@@ -1569,7 +1573,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="15"/>
       <c r="B5" t="s">
         <v>182</v>
       </c>
@@ -1579,7 +1583,7 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
@@ -1613,7 +1617,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="15"/>
       <c r="B6" t="s">
         <v>183</v>
       </c>
@@ -1623,7 +1627,7 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>3</v>
       </c>
       <c r="F6" t="s">
@@ -1657,7 +1661,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="15"/>
       <c r="B7" t="s">
         <v>184</v>
       </c>
@@ -1667,7 +1671,7 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>1</v>
       </c>
       <c r="F7" t="s">
@@ -1701,7 +1705,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="15"/>
       <c r="B8" t="s">
         <v>185</v>
       </c>
@@ -1711,7 +1715,7 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>1</v>
       </c>
       <c r="F8" t="s">
@@ -1745,7 +1749,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="15"/>
       <c r="B9" t="s">
         <v>186</v>
       </c>
@@ -1755,7 +1759,7 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>1</v>
       </c>
       <c r="F9" t="s">
@@ -1789,7 +1793,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="15"/>
       <c r="B10" t="s">
         <v>187</v>
       </c>
@@ -1799,7 +1803,7 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>2</v>
       </c>
       <c r="F10" t="s">
@@ -1833,7 +1837,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="15"/>
       <c r="B11" t="s">
         <v>188</v>
       </c>
@@ -1843,7 +1847,7 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>1</v>
       </c>
       <c r="F11" t="s">
@@ -1861,7 +1865,7 @@
       <c r="J11" t="s">
         <v>143</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="11" t="s">
         <v>289</v>
       </c>
       <c r="L11" s="2">
@@ -1878,7 +1882,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="15"/>
       <c r="B12" t="s">
         <v>189</v>
       </c>
@@ -1888,7 +1892,7 @@
       <c r="D12" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>1</v>
       </c>
       <c r="F12" t="s">
@@ -1923,7 +1927,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="15"/>
       <c r="B13" t="s">
         <v>190</v>
       </c>
@@ -1933,7 +1937,7 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>5</v>
       </c>
       <c r="F13" t="s">
@@ -1967,7 +1971,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="15"/>
       <c r="B14" t="s">
         <v>191</v>
       </c>
@@ -1977,7 +1981,7 @@
       <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>4</v>
       </c>
       <c r="F14" t="s">
@@ -2011,7 +2015,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="15"/>
       <c r="B15" t="s">
         <v>192</v>
       </c>
@@ -2021,7 +2025,7 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="5">
         <v>1</v>
       </c>
       <c r="F15" t="s">
@@ -2055,7 +2059,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="14"/>
       <c r="B16" t="s">
         <v>193</v>
       </c>
@@ -2065,7 +2069,7 @@
       <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="5">
         <v>1</v>
       </c>
       <c r="F16" t="s">
@@ -2099,7 +2103,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="14"/>
       <c r="B17" t="s">
         <v>194</v>
       </c>
@@ -2109,7 +2113,7 @@
       <c r="D17" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>1</v>
       </c>
       <c r="F17" t="s">
@@ -2143,7 +2147,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="14"/>
       <c r="B18" t="s">
         <v>195</v>
       </c>
@@ -2153,7 +2157,7 @@
       <c r="D18" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <v>1</v>
       </c>
       <c r="F18" t="s">
@@ -2187,7 +2191,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="14"/>
       <c r="B19" t="s">
         <v>229</v>
       </c>
@@ -2197,7 +2201,7 @@
       <c r="D19" t="s">
         <v>168</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>1</v>
       </c>
       <c r="F19" t="s">
@@ -2231,7 +2235,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="14"/>
       <c r="B20" t="s">
         <v>230</v>
       </c>
@@ -2241,7 +2245,7 @@
       <c r="D20" t="s">
         <v>165</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <v>3</v>
       </c>
       <c r="F20" t="s">
@@ -2276,7 +2280,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="14"/>
       <c r="B21" t="s">
         <v>231</v>
       </c>
@@ -2286,7 +2290,7 @@
       <c r="D21" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <v>1</v>
       </c>
       <c r="F21" t="s">
@@ -2321,7 +2325,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="14"/>
       <c r="B22" t="s">
         <v>232</v>
       </c>
@@ -2331,7 +2335,7 @@
       <c r="D22" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <v>1</v>
       </c>
       <c r="F22" t="s">
@@ -2367,7 +2371,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="14"/>
       <c r="B23" t="s">
         <v>233</v>
       </c>
@@ -2377,7 +2381,7 @@
       <c r="D23" t="s">
         <v>167</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <v>1</v>
       </c>
       <c r="F23" t="s">
@@ -2413,7 +2417,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="14"/>
       <c r="B24" t="s">
         <v>234</v>
       </c>
@@ -2423,7 +2427,7 @@
       <c r="D24" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <v>4</v>
       </c>
       <c r="F24" t="s">
@@ -2457,7 +2461,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="14"/>
       <c r="B25" t="s">
         <v>235</v>
       </c>
@@ -2467,7 +2471,7 @@
       <c r="D25" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>5</v>
       </c>
       <c r="F25" t="s">
@@ -2501,7 +2505,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="14"/>
       <c r="B26" t="s">
         <v>236</v>
       </c>
@@ -2511,7 +2515,7 @@
       <c r="D26" t="s">
         <v>114</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="5">
         <v>1</v>
       </c>
       <c r="F26" t="s">
@@ -2545,7 +2549,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="14"/>
       <c r="B27" t="s">
         <v>237</v>
       </c>
@@ -2555,7 +2559,7 @@
       <c r="D27" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="5">
         <v>3</v>
       </c>
       <c r="F27" t="s">
@@ -2589,7 +2593,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="14"/>
       <c r="B28" t="s">
         <v>238</v>
       </c>
@@ -2599,7 +2603,7 @@
       <c r="D28" t="s">
         <v>129</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="5">
         <v>25</v>
       </c>
       <c r="F28" t="s">
@@ -2633,7 +2637,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="14"/>
       <c r="B29" t="s">
         <v>239</v>
       </c>
@@ -2643,7 +2647,7 @@
       <c r="D29" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="5">
         <v>2</v>
       </c>
       <c r="F29" t="s">
@@ -2679,7 +2683,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="14"/>
       <c r="B30" t="s">
         <v>240</v>
       </c>
@@ -2689,7 +2693,7 @@
       <c r="D30" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="5">
         <v>1</v>
       </c>
       <c r="F30" t="s">
@@ -2725,7 +2729,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="14"/>
       <c r="B31" t="s">
         <v>241</v>
       </c>
@@ -2735,7 +2739,7 @@
       <c r="D31" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="5">
         <v>1</v>
       </c>
       <c r="F31" t="s">
@@ -2771,7 +2775,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="14"/>
       <c r="B32" t="s">
         <v>242</v>
       </c>
@@ -2781,7 +2785,7 @@
       <c r="D32" t="s">
         <v>206</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="5">
         <v>1</v>
       </c>
       <c r="F32" t="s">
@@ -2815,7 +2819,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="14"/>
       <c r="B33" t="s">
         <v>284</v>
       </c>
@@ -2825,7 +2829,7 @@
       <c r="D33" t="s">
         <v>114</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="5">
         <v>1</v>
       </c>
       <c r="F33" t="s">
@@ -2859,7 +2863,7 @@
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="14"/>
       <c r="B34" t="s">
         <v>285</v>
       </c>
@@ -2869,7 +2873,7 @@
       <c r="D34" t="s">
         <v>114</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="5">
         <v>2</v>
       </c>
       <c r="F34" t="s">
@@ -2903,7 +2907,7 @@
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="14"/>
       <c r="B35" t="s">
         <v>286</v>
       </c>
@@ -2913,7 +2917,7 @@
       <c r="D35" t="s">
         <v>129</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="5">
         <v>15</v>
       </c>
       <c r="F35" t="s">
@@ -2947,24 +2951,24 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="10"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="7"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B37" t="s">
@@ -2976,7 +2980,7 @@
       <c r="D37" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="5">
         <v>1</v>
       </c>
       <c r="F37" t="s">
@@ -3005,7 +3009,7 @@
       <c r="N37" s="2"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="14"/>
       <c r="B38" t="s">
         <v>49</v>
       </c>
@@ -3015,7 +3019,7 @@
       <c r="D38" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="5">
         <v>1</v>
       </c>
       <c r="F38" t="s">
@@ -3044,7 +3048,7 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+      <c r="A39" s="14"/>
       <c r="B39" t="s">
         <v>50</v>
       </c>
@@ -3054,7 +3058,7 @@
       <c r="D39" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="5">
         <v>3</v>
       </c>
       <c r="F39" t="s">
@@ -3083,7 +3087,7 @@
       <c r="N39" s="2"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="14"/>
       <c r="B40" t="s">
         <v>51</v>
       </c>
@@ -3093,7 +3097,7 @@
       <c r="D40" t="s">
         <v>1</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="5">
         <v>3</v>
       </c>
       <c r="F40" t="s">
@@ -3122,7 +3126,7 @@
       <c r="N40" s="2"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="14"/>
       <c r="B41" t="s">
         <v>52</v>
       </c>
@@ -3132,7 +3136,7 @@
       <c r="D41" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="5">
         <v>1</v>
       </c>
       <c r="F41" t="s">
@@ -3161,7 +3165,7 @@
       <c r="N41" s="2"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="14"/>
       <c r="B42" t="s">
         <v>53</v>
       </c>
@@ -3171,7 +3175,7 @@
       <c r="D42" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="5">
         <v>1</v>
       </c>
       <c r="F42" t="s">
@@ -3200,7 +3204,7 @@
       <c r="N42" s="2"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
+      <c r="A43" s="14"/>
       <c r="B43" t="s">
         <v>54</v>
       </c>
@@ -3210,7 +3214,7 @@
       <c r="D43" t="s">
         <v>1</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="5">
         <v>1</v>
       </c>
       <c r="F43" t="s">
@@ -3239,7 +3243,7 @@
       <c r="N43" s="2"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
+      <c r="A44" s="14"/>
       <c r="B44" t="s">
         <v>55</v>
       </c>
@@ -3249,7 +3253,7 @@
       <c r="D44" t="s">
         <v>1</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="5">
         <v>1</v>
       </c>
       <c r="F44" t="s">
@@ -3278,7 +3282,7 @@
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
+      <c r="A45" s="14"/>
       <c r="B45" t="s">
         <v>56</v>
       </c>
@@ -3288,7 +3292,7 @@
       <c r="D45" t="s">
         <v>1</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="5">
         <v>1</v>
       </c>
       <c r="F45" t="s">
@@ -3317,7 +3321,7 @@
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
+      <c r="A46" s="14"/>
       <c r="B46" t="s">
         <v>57</v>
       </c>
@@ -3327,7 +3331,7 @@
       <c r="D46" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="5">
         <v>1</v>
       </c>
       <c r="F46" t="s">
@@ -3356,7 +3360,7 @@
       <c r="N46" s="2"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
+      <c r="A47" s="14"/>
       <c r="B47" t="s">
         <v>58</v>
       </c>
@@ -3366,7 +3370,7 @@
       <c r="D47" t="s">
         <v>1</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="5">
         <v>2</v>
       </c>
       <c r="F47" t="s">
@@ -3395,7 +3399,7 @@
       <c r="N47" s="2"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
+      <c r="A48" s="14"/>
       <c r="B48" t="s">
         <v>59</v>
       </c>
@@ -3405,7 +3409,7 @@
       <c r="D48" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="5">
         <v>1</v>
       </c>
       <c r="F48" t="s">
@@ -3434,7 +3438,7 @@
       <c r="N48" s="2"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
+      <c r="A49" s="14"/>
       <c r="B49" t="s">
         <v>60</v>
       </c>
@@ -3444,7 +3448,7 @@
       <c r="D49" t="s">
         <v>38</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="5">
         <v>6</v>
       </c>
       <c r="F49" t="s">
@@ -3473,7 +3477,7 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
+      <c r="A50" s="14"/>
       <c r="B50" t="s">
         <v>61</v>
       </c>
@@ -3483,7 +3487,7 @@
       <c r="D50" t="s">
         <v>38</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50" s="5">
         <v>6</v>
       </c>
       <c r="F50" t="s">
@@ -3512,7 +3516,7 @@
       <c r="N50" s="2"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
+      <c r="A51" s="14"/>
       <c r="B51" t="s">
         <v>62</v>
       </c>
@@ -3522,7 +3526,7 @@
       <c r="D51" t="s">
         <v>38</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="5">
         <v>3</v>
       </c>
       <c r="F51" t="s">
@@ -3551,7 +3555,7 @@
       <c r="N51" s="2"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
+      <c r="A52" s="14"/>
       <c r="B52" t="s">
         <v>199</v>
       </c>
@@ -3561,8 +3565,8 @@
       <c r="D52" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="7">
-        <v>8</v>
+      <c r="E52" s="5">
+        <v>12</v>
       </c>
       <c r="F52" t="s">
         <v>76</v>
@@ -3590,7 +3594,7 @@
       <c r="N52" s="2"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
+      <c r="A53" s="14"/>
       <c r="B53" t="s">
         <v>200</v>
       </c>
@@ -3600,8 +3604,8 @@
       <c r="D53" t="s">
         <v>40</v>
       </c>
-      <c r="E53" s="7">
-        <v>5</v>
+      <c r="E53" s="5">
+        <v>4</v>
       </c>
       <c r="F53" t="s">
         <v>76</v>
@@ -3626,7 +3630,7 @@
       <c r="N53" s="2"/>
     </row>
     <row r="54" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
+      <c r="A54" s="14"/>
       <c r="B54" t="s">
         <v>201</v>
       </c>
@@ -3636,7 +3640,7 @@
       <c r="D54" t="s">
         <v>41</v>
       </c>
-      <c r="E54" s="7">
+      <c r="E54" s="5">
         <v>2</v>
       </c>
       <c r="F54" t="s">
@@ -3659,7 +3663,7 @@
       <c r="N54" s="2"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
+      <c r="A55" s="14"/>
       <c r="B55" t="s">
         <v>260</v>
       </c>
@@ -3669,7 +3673,7 @@
       <c r="D55" t="s">
         <v>262</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E55" s="5">
         <v>1</v>
       </c>
       <c r="F55" t="s">
@@ -3695,12 +3699,12 @@
       <c r="N56" s="2"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="13" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
+      <c r="A59" s="13"/>
       <c r="B59" t="s">
         <v>179</v>
       </c>
@@ -3710,7 +3714,7 @@
       <c r="D59" t="s">
         <v>172</v>
       </c>
-      <c r="E59" s="7">
+      <c r="E59" s="5">
         <v>1</v>
       </c>
       <c r="F59" t="s">
@@ -3744,7 +3748,7 @@
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
+      <c r="A60" s="13"/>
       <c r="B60" t="s">
         <v>180</v>
       </c>
@@ -3754,7 +3758,7 @@
       <c r="D60" t="s">
         <v>177</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60" s="5">
         <v>1</v>
       </c>
       <c r="F60" t="s">
@@ -3788,7 +3792,7 @@
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
+      <c r="A61" s="13"/>
       <c r="L61" s="2"/>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>

</xml_diff>